<commit_message>
Added annotations to BOMs
 * Note what we already had parts for
 * Note what we had to order a replacement part for from digikey (some stuff was out of stock)
</commit_message>
<xml_diff>
--- a/modules/audio_spectrum/rev_a/audio_spectrum_bom.xlsx
+++ b/modules/audio_spectrum/rev_a/audio_spectrum_bom.xlsx
@@ -652,7 +652,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -662,6 +662,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,18 +689,18 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q52" activeCellId="0" sqref="Q52"/>
+      <selection pane="topLeft" activeCell="F71" activeCellId="0" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,27 +1513,26 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">

</xml_diff>